<commit_message>
corrected SMC in BSM
</commit_message>
<xml_diff>
--- a/SCOPE_v1.71/input_data.xlsx
+++ b/SCOPE_v1.71/input_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="5568" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8892" windowHeight="5196" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="5" r:id="rId1"/>
@@ -3102,7 +3102,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
corrected SMC in time series: required as one column file in both .xlsx and .m versions of input
</commit_message>
<xml_diff>
--- a/SCOPE_v1.71/input_data.xlsx
+++ b/SCOPE_v1.71/input_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8892" windowHeight="5196" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8892" windowHeight="5196" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="347">
   <si>
     <t>Cab</t>
   </si>
@@ -1267,12 +1267,15 @@
   <si>
     <t>optiona_leaf_inclination_distribution_file_with_3_headerlines._MUST_be_located_in_../data/leafangles/</t>
   </si>
+  <si>
+    <t>optional_(leave_empty_for_calculations_based_on_t_file_year_timezn)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1410,6 +1413,15 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1600,7 +1612,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1707,6 +1719,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3342,10 +3355,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3487,56 +3500,61 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="56" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="50" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="50" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="49"/>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="49"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>